<commit_message>
Fixed bug on Neonatal mortality data
</commit_message>
<xml_diff>
--- a/data/indicator_data.xlsx
+++ b/data/indicator_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="25360" windowHeight="14200" tabRatio="500"/>
+    <workbookView xWindow="60" yWindow="0" windowWidth="25360" windowHeight="14200" tabRatio="500" firstSheet="2" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="22" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="3_2" sheetId="7" r:id="rId8"/>
     <sheet name="3_3" sheetId="8" r:id="rId9"/>
     <sheet name="4_1" sheetId="9" r:id="rId10"/>
-    <sheet name="4_2" sheetId="10" r:id="rId11"/>
+    <sheet name="4_2" sheetId="23" r:id="rId11"/>
     <sheet name="5_1" sheetId="11" r:id="rId12"/>
     <sheet name="5_2" sheetId="12" r:id="rId13"/>
     <sheet name="5_3" sheetId="13" r:id="rId14"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="107">
   <si>
     <t>Year</t>
   </si>
@@ -77,22 +77,10 @@
     <t>2014-15</t>
   </si>
   <si>
-    <t>Labor force participation rate, female (% of female population ages 15+) (national estimate)</t>
-  </si>
-  <si>
-    <t>Labor force participation rate, male (% of male population ages 15+) (national estimate)</t>
-  </si>
-  <si>
-    <t>Labor force participation rate, total (% of total population ages 15+) (national estimate)</t>
-  </si>
-  <si>
     <t>Infant mortality rate</t>
   </si>
   <si>
     <t>Neonatal mortality rate</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>Deaths per 100,000 births</t>
@@ -380,8 +368,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="#.00;\-#.00;0.00;@"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="#.00;\-#.00;0.00;@"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -494,7 +482,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="100">
+  <cellStyleXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -518,7 +506,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -596,7 +586,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -606,8 +596,8 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -622,7 +612,7 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="23" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="23" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -638,11 +628,14 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="100">
+  <cellStyles count="102">
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
@@ -691,6 +684,7 @@
     <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -739,6 +733,7 @@
     <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="23"/>
@@ -1073,7 +1068,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1085,354 +1080,354 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B16" s="16"/>
       <c r="D16" s="15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C20" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="E20" s="15" t="s">
         <v>102</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B21" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="D21" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="C21" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>108</v>
-      </c>
       <c r="E21" s="15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1469,7 +1464,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1482,11 +1477,11 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="1">
+      <c r="A2" s="20">
         <v>2002</v>
       </c>
       <c r="B2" s="5">
@@ -1494,7 +1489,7 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="1">
+      <c r="A3" s="20">
         <v>2003</v>
       </c>
       <c r="B3" s="5">
@@ -1502,7 +1497,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="1">
+      <c r="A4" s="20">
         <v>2004</v>
       </c>
       <c r="B4" s="5">
@@ -1510,7 +1505,7 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="1">
+      <c r="A5" s="20">
         <v>2005</v>
       </c>
       <c r="B5" s="5">
@@ -1518,7 +1513,7 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="1">
+      <c r="A6" s="20">
         <v>2006</v>
       </c>
       <c r="B6" s="5">
@@ -1526,7 +1521,7 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="1">
+      <c r="A7" s="20">
         <v>2007</v>
       </c>
       <c r="B7" s="5">
@@ -1534,7 +1529,7 @@
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="1">
+      <c r="A8" s="20">
         <v>2008</v>
       </c>
       <c r="B8" s="5">
@@ -1542,7 +1537,7 @@
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="1">
+      <c r="A9" s="20">
         <v>2009</v>
       </c>
       <c r="B9" s="5">
@@ -1550,7 +1545,7 @@
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="1">
+      <c r="A10" s="20">
         <v>2010</v>
       </c>
       <c r="B10" s="5">
@@ -1558,7 +1553,7 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="1">
+      <c r="A11" s="20">
         <v>2011</v>
       </c>
       <c r="B11" s="5">
@@ -1566,7 +1561,7 @@
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="1">
+      <c r="A12" s="20">
         <v>2012</v>
       </c>
       <c r="B12" s="5">
@@ -1586,24 +1581,27 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="12.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="1">
+      <c r="A2" s="20">
         <v>2002</v>
       </c>
       <c r="B2" s="5">
@@ -1611,7 +1609,7 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="1">
+      <c r="A3" s="20">
         <v>2003</v>
       </c>
       <c r="B3" s="5">
@@ -1619,7 +1617,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="1">
+      <c r="A4" s="20">
         <v>2004</v>
       </c>
       <c r="B4" s="6">
@@ -1628,7 +1626,7 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="1">
+      <c r="A5" s="20">
         <v>2005</v>
       </c>
       <c r="B5" s="5">
@@ -1636,7 +1634,7 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="1">
+      <c r="A6" s="20">
         <v>2006</v>
       </c>
       <c r="B6" s="5">
@@ -1644,7 +1642,7 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="1">
+      <c r="A7" s="20">
         <v>2007</v>
       </c>
       <c r="B7" s="5">
@@ -1652,7 +1650,7 @@
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="1">
+      <c r="A8" s="20">
         <v>2008</v>
       </c>
       <c r="B8" s="5">
@@ -1660,7 +1658,7 @@
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="1">
+      <c r="A9" s="20">
         <v>2009</v>
       </c>
       <c r="B9" s="6">
@@ -1669,7 +1667,7 @@
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="1">
+      <c r="A10" s="20">
         <v>2010</v>
       </c>
       <c r="B10" s="6">
@@ -1678,17 +1676,11 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="1">
+      <c r="A11" s="20">
         <v>2011</v>
       </c>
       <c r="B11" s="5">
         <v>11.1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="1"/>
-      <c r="B12" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1706,8 +1698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1721,7 +1713,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1838,7 +1830,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="12" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B1" s="14">
         <v>2003</v>
@@ -1849,7 +1841,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="13" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B2" s="19">
         <v>90.8</v>
@@ -1860,7 +1852,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="13" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B3" s="19">
         <v>97</v>
@@ -1871,7 +1863,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="13" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B4" s="19">
         <v>97.8</v>
@@ -1882,7 +1874,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="13" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B5" s="19">
         <v>96.2</v>
@@ -1893,7 +1885,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B6" s="19">
         <v>97.6</v>
@@ -1904,7 +1896,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="13" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B7" s="19">
         <v>98.7</v>
@@ -1915,7 +1907,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="13" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B8" s="19">
         <v>96.2</v>
@@ -1926,7 +1918,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="13" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B9" s="19">
         <v>97.2</v>
@@ -1961,7 +1953,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="12" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B1" s="14">
         <v>2003</v>
@@ -1972,7 +1964,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="13" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B2" s="19">
         <v>1.7000000000000002</v>
@@ -1983,7 +1975,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="13" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B3" s="19">
         <v>12.3</v>
@@ -1994,7 +1986,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="13" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B4" s="19">
         <v>34.799999999999997</v>
@@ -2005,7 +1997,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="13" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B5" s="19">
         <v>44.800000000000004</v>
@@ -2016,7 +2008,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B6" s="19">
         <v>64.099999999999994</v>
@@ -2027,7 +2019,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="13" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B7" s="19">
         <v>56.2</v>
@@ -2038,7 +2030,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="13" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B8" s="19">
         <v>53.800000000000004</v>
@@ -2049,7 +2041,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="13" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B9" s="19">
         <v>35</v>
@@ -2090,13 +2082,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2214,7 +2206,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2298,10 +2290,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2461,15 +2453,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B2">
         <v>1800</v>
@@ -2477,7 +2469,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <v>13</v>
@@ -2485,7 +2477,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B4">
         <v>250</v>
@@ -2493,7 +2485,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B5">
         <v>200</v>
@@ -2501,7 +2493,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B6">
         <v>500</v>
@@ -2536,7 +2528,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2642,7 +2634,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2766,7 +2758,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2909,13 +2901,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3118,7 +3110,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3262,13 +3254,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3367,13 +3359,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3567,16 +3559,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -3782,7 +3774,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3794,14 +3786,14 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>14</v>
+      <c r="B1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3994,7 +3986,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4004,13 +3996,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4">

</xml_diff>

<commit_message>
Added custom line colors for all charts
</commit_message>
<xml_diff>
--- a/data/indicator_data.xlsx
+++ b/data/indicator_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="25360" windowHeight="14200" tabRatio="500" firstSheet="2" activeTab="11"/>
+    <workbookView xWindow="60" yWindow="0" windowWidth="25360" windowHeight="14200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="22" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="147">
   <si>
     <t>Year</t>
   </si>
@@ -185,18 +185,12 @@
     <t>Years</t>
   </si>
   <si>
-    <t>Life expectancy at birth</t>
-  </si>
-  <si>
     <t>3_3</t>
   </si>
   <si>
     <t>% of population ages 15+</t>
   </si>
   <si>
-    <t>Labor force participation rates (National Estimate)</t>
-  </si>
-  <si>
     <t>3_2</t>
   </si>
   <si>
@@ -230,18 +224,12 @@
     <t>1_3</t>
   </si>
   <si>
-    <t>Employment to population ratios</t>
-  </si>
-  <si>
     <t>1_2</t>
   </si>
   <si>
     <t>% of the population</t>
   </si>
   <si>
-    <t>Poverty headcount ratio at national poverty lines</t>
-  </si>
-  <si>
     <t>1_1</t>
   </si>
   <si>
@@ -360,6 +348,138 @@
   </si>
   <si>
     <t>_</t>
+  </si>
+  <si>
+    <t>bg_color</t>
+  </si>
+  <si>
+    <t>#FCDB32</t>
+  </si>
+  <si>
+    <t>#D6DD3A</t>
+  </si>
+  <si>
+    <t>#F3941D</t>
+  </si>
+  <si>
+    <t>#C7EBFC</t>
+  </si>
+  <si>
+    <t>#F6C2DA</t>
+  </si>
+  <si>
+    <t>#EE5B45</t>
+  </si>
+  <si>
+    <t>#8CC449</t>
+  </si>
+  <si>
+    <t>#29B1E6</t>
+  </si>
+  <si>
+    <t>line_color_1</t>
+  </si>
+  <si>
+    <t>line_color_2</t>
+  </si>
+  <si>
+    <t>line_color_3</t>
+  </si>
+  <si>
+    <t>#191500</t>
+  </si>
+  <si>
+    <t>#E15554</t>
+  </si>
+  <si>
+    <t>#4D9DE0</t>
+  </si>
+  <si>
+    <t>Poverty Headcount Ratio at National Poverty Lines</t>
+  </si>
+  <si>
+    <t>Employment to Population Ratios</t>
+  </si>
+  <si>
+    <t>GDP per Capita</t>
+  </si>
+  <si>
+    <t>Labor Force Participation Rates (National Estimate)</t>
+  </si>
+  <si>
+    <t>Life Expectancy at Birth</t>
+  </si>
+  <si>
+    <t>Infant Mortality Rate</t>
+  </si>
+  <si>
+    <t>Neonatal Mortality Rate</t>
+  </si>
+  <si>
+    <t>#247BA0</t>
+  </si>
+  <si>
+    <t>#F25F5C</t>
+  </si>
+  <si>
+    <t>#50514F</t>
+  </si>
+  <si>
+    <t>line_color_4</t>
+  </si>
+  <si>
+    <t>#E4FDE1</t>
+  </si>
+  <si>
+    <t>#8ACB88</t>
+  </si>
+  <si>
+    <t>#648381</t>
+  </si>
+  <si>
+    <t>#575761</t>
+  </si>
+  <si>
+    <t>#C95D63</t>
+  </si>
+  <si>
+    <t>#496DDB</t>
+  </si>
+  <si>
+    <t>#3A3042</t>
+  </si>
+  <si>
+    <t>#1C1D21</t>
+  </si>
+  <si>
+    <t>#746D75</t>
+  </si>
+  <si>
+    <t>#412B2B</t>
+  </si>
+  <si>
+    <t>#313930</t>
+  </si>
+  <si>
+    <t>#BEBBBB</t>
+  </si>
+  <si>
+    <t>#444054</t>
+  </si>
+  <si>
+    <t>#2F243A</t>
+  </si>
+  <si>
+    <t>#000B28</t>
+  </si>
+  <si>
+    <t>#C69FB1</t>
+  </si>
+  <si>
+    <t>#80CED7</t>
+  </si>
+  <si>
+    <t>#263D42</t>
   </si>
 </sst>
 </file>
@@ -482,7 +602,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="102">
+  <cellStyleXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -507,6 +627,42 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="166" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -635,7 +791,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="102">
+  <cellStyles count="138">
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
@@ -685,6 +841,24 @@
     <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -734,6 +908,24 @@
     <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="23"/>
@@ -1066,386 +1258,614 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="42" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:10">
       <c r="A1" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="G1" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>66</v>
+        <v>118</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D2" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="J3" s="15"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="J5" s="15"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="J6" s="15"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="F7" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="G7" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="J7" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="15" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" s="15" t="s">
+      <c r="E8" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="E3" s="15" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="G8" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="J8" s="15"/>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>48</v>
+        <v>122</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>47</v>
       </c>
       <c r="D9" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="F9" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="E9" s="15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="G9" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="J9" s="15"/>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>46</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>12</v>
+        <v>123</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>102</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>45</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>13</v>
+        <v>124</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>102</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>102</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B13" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C15" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="D13" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="E13" s="15" t="s">
+      <c r="D15" s="15" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>73</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="E14" s="15" t="s">
+      <c r="E15" s="15" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
-        <v>74</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="J15" s="15"/>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B16" s="16"/>
       <c r="D16" s="15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>102</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" t="s">
         <v>76</v>
       </c>
-      <c r="B17" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
-        <v>77</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="E18" s="15" t="s">
+      <c r="B21" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="E21" s="15" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" t="s">
-        <v>78</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="s">
-        <v>79</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" t="s">
-        <v>80</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="F21" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+    </row>
+    <row r="22" spans="1:10">
       <c r="B22" s="16"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:10">
       <c r="B23" s="16"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:10">
       <c r="B24" s="16"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:10">
       <c r="B25" s="16"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:10">
       <c r="B26" s="16"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:10">
       <c r="B27" s="16"/>
     </row>
   </sheetData>
@@ -1698,8 +2118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2206,7 +2626,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2290,10 +2710,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2456,7 +2876,7 @@
         <v>28</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2634,7 +3054,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3346,29 +3766,26 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -3378,12 +3795,8 @@
       <c r="C2">
         <v>156566</v>
       </c>
-      <c r="D2">
-        <f>B2+C2</f>
-        <v>327207</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -3393,12 +3806,8 @@
       <c r="C3">
         <v>154728</v>
       </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D12" si="0">B3+C3</f>
-        <v>322180</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -3408,12 +3817,8 @@
       <c r="C4">
         <v>156210</v>
       </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>324614</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -3423,12 +3828,8 @@
       <c r="C5">
         <v>157639</v>
       </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>326911</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -3438,12 +3839,8 @@
       <c r="C6">
         <v>153669</v>
       </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>322975</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -3453,12 +3850,8 @@
       <c r="C7">
         <v>149217</v>
       </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>311744</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -3468,12 +3861,8 @@
       <c r="C8">
         <v>145516</v>
       </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>301486</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -3483,12 +3872,8 @@
       <c r="C9">
         <v>142806</v>
       </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>295218</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -3498,12 +3883,8 @@
       <c r="C10">
         <v>142806</v>
       </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>295218</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -3513,12 +3894,8 @@
       <c r="C11">
         <v>134273</v>
       </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>278608</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -3527,10 +3904,6 @@
       </c>
       <c r="C12">
         <v>132481</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>273649</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added column chart option
</commit_message>
<xml_diff>
--- a/data/indicator_data.xlsx
+++ b/data/indicator_data.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="145">
   <si>
     <t>Year</t>
   </si>
@@ -116,9 +116,6 @@
     <t>AIDS</t>
   </si>
   <si>
-    <t>AIDS/HIV</t>
-  </si>
-  <si>
     <t>HIV</t>
   </si>
   <si>
@@ -296,9 +293,6 @@
     <t>Area</t>
   </si>
   <si>
-    <t>Area in hectares</t>
-  </si>
-  <si>
     <t>Afforested Area</t>
   </si>
   <si>
@@ -455,9 +449,6 @@
     <t>#746D75</t>
   </si>
   <si>
-    <t>#412B2B</t>
-  </si>
-  <si>
     <t>#313930</t>
   </si>
   <si>
@@ -470,16 +461,19 @@
     <t>#2F243A</t>
   </si>
   <si>
-    <t>#000B28</t>
-  </si>
-  <si>
-    <t>#C69FB1</t>
-  </si>
-  <si>
     <t>#80CED7</t>
   </si>
   <si>
     <t>#263D42</t>
+  </si>
+  <si>
+    <t>#F2F7F2</t>
+  </si>
+  <si>
+    <t>#443850</t>
+  </si>
+  <si>
+    <t>Cumulative Area in hectares</t>
   </si>
 </sst>
 </file>
@@ -602,7 +596,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="138">
+  <cellStyleXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -627,6 +621,26 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="166" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -791,7 +805,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="138">
+  <cellStyles count="158">
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
@@ -859,6 +873,16 @@
     <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -926,6 +950,16 @@
     <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="150" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="152" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="154" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="156" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="23"/>
@@ -1261,7 +1295,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14:H14"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1273,57 +1307,57 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G1" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="I1" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="H1" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>114</v>
-      </c>
       <c r="J1" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D2" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="F2" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="E2" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>104</v>
-      </c>
       <c r="G2" s="15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H2" s="15"/>
       <c r="I2" s="15"/>
@@ -1331,55 +1365,55 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="E3" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>104</v>
-      </c>
       <c r="G3" s="15" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J3" s="15"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="E4" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="F4" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="F4" s="15" t="s">
-        <v>104</v>
-      </c>
       <c r="G4" s="15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
@@ -1387,177 +1421,177 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G5" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="I5" s="15" t="s">
         <v>125</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>127</v>
       </c>
       <c r="J5" s="15"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G6" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="I6" s="15" t="s">
         <v>125</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="I6" s="15" t="s">
-        <v>127</v>
       </c>
       <c r="J6" s="15"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G7" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="I7" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="J7" s="15" t="s">
         <v>130</v>
-      </c>
-      <c r="I7" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="J7" s="15" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G8" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="I8" s="15" t="s">
         <v>133</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="I8" s="15" t="s">
-        <v>135</v>
       </c>
       <c r="J8" s="15"/>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G9" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="I9" s="15" t="s">
         <v>133</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="I9" s="15" t="s">
-        <v>135</v>
       </c>
       <c r="J9" s="15"/>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H10" s="15"/>
       <c r="I10" s="15"/>
@@ -1565,25 +1599,25 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
@@ -1591,25 +1625,25 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H12" s="15"/>
       <c r="I12" s="15"/>
@@ -1617,103 +1651,103 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B13" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="C13" s="15" t="s">
-        <v>79</v>
-      </c>
       <c r="D13" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="I13" s="15"/>
       <c r="J13" s="15"/>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="I14" s="15"/>
       <c r="J14" s="15"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B15" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="C15" s="18" t="s">
-        <v>83</v>
-      </c>
       <c r="D15" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="J15" s="15"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B16" s="16"/>
       <c r="D16" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
@@ -1722,25 +1756,25 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>85</v>
+        <v>144</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="H17" s="15"/>
       <c r="I17" s="15"/>
@@ -1748,77 +1782,79 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G18" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="H18" s="15" t="s">
         <v>143</v>
-      </c>
-      <c r="H18" s="15" t="s">
-        <v>144</v>
       </c>
       <c r="I18" s="15"/>
       <c r="J18" s="15"/>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="G19" s="15"/>
+        <v>108</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>142</v>
+      </c>
       <c r="H19" s="15"/>
       <c r="I19" s="15"/>
       <c r="J19" s="15"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="H20" s="15"/>
       <c r="I20" s="15"/>
@@ -1826,25 +1862,25 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D21" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="E21" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="E21" s="15" t="s">
-        <v>102</v>
-      </c>
       <c r="F21" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="H21" s="15"/>
       <c r="I21" s="15"/>
@@ -2483,35 +2519,30 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="6.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="1">
         <v>2010</v>
       </c>
@@ -2521,11 +2552,8 @@
       <c r="C2">
         <v>3</v>
       </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="1">
         <v>2011</v>
       </c>
@@ -2535,11 +2563,8 @@
       <c r="C3">
         <v>7</v>
       </c>
-      <c r="D3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="1">
         <v>2012</v>
       </c>
@@ -2549,11 +2574,8 @@
       <c r="C4">
         <v>2</v>
       </c>
-      <c r="D4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="1">
         <v>2013</v>
       </c>
@@ -2563,11 +2585,8 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="1">
         <v>2014</v>
       </c>
@@ -2576,9 +2595,6 @@
       </c>
       <c r="C6">
         <v>1</v>
-      </c>
-      <c r="D6">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -2616,7 +2632,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2626,7 +2642,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2710,10 +2726,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2873,15 +2889,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2">
         <v>1800</v>
@@ -2889,7 +2905,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3">
         <v>13</v>
@@ -2897,7 +2913,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4">
         <v>250</v>
@@ -2905,7 +2921,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5">
         <v>200</v>
@@ -2913,7 +2929,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6">
         <v>500</v>
@@ -2948,7 +2964,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -3054,7 +3070,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3178,7 +3194,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3321,13 +3337,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3530,7 +3546,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3674,13 +3690,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>38</v>
-      </c>
       <c r="D1" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3779,10 +3795,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -3932,16 +3948,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -4160,13 +4176,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -4369,13 +4385,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4">

</xml_diff>

<commit_message>
Added data verification document
</commit_message>
<xml_diff>
--- a/data/indicator_data.xlsx
+++ b/data/indicator_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19340" windowHeight="14340" tabRatio="854"/>
+    <workbookView xWindow="48020" yWindow="0" windowWidth="15920" windowHeight="21100" tabRatio="854"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="22" r:id="rId1"/>
@@ -19,16 +19,14 @@
     <sheet name="3_4" sheetId="24" r:id="rId10"/>
     <sheet name="4_1" sheetId="9" r:id="rId11"/>
     <sheet name="4_2" sheetId="23" r:id="rId12"/>
-    <sheet name="5_2" sheetId="12" r:id="rId13"/>
-    <sheet name="5_1" sheetId="11" r:id="rId14"/>
+    <sheet name="5_1" sheetId="11" r:id="rId13"/>
+    <sheet name="5_2" sheetId="12" r:id="rId14"/>
     <sheet name="5_3" sheetId="13" r:id="rId15"/>
     <sheet name="6_1" sheetId="14" r:id="rId16"/>
-    <sheet name="6_2" sheetId="15" r:id="rId17"/>
-    <sheet name="7_1" sheetId="16" r:id="rId18"/>
-    <sheet name="7_2" sheetId="20" r:id="rId19"/>
-    <sheet name="7_3" sheetId="17" r:id="rId20"/>
-    <sheet name="8_1" sheetId="18" r:id="rId21"/>
-    <sheet name="8_2" sheetId="19" r:id="rId22"/>
+    <sheet name="7_1" sheetId="16" r:id="rId17"/>
+    <sheet name="7_2" sheetId="20" r:id="rId18"/>
+    <sheet name="7_3" sheetId="17" r:id="rId19"/>
+    <sheet name="8_1" sheetId="18" r:id="rId20"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -40,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="150">
   <si>
     <t>Year</t>
   </si>
@@ -138,9 +136,6 @@
     <t>Species of Aquatic Macrobenthos</t>
   </si>
   <si>
-    <t>Use of IMF credit (DOD, current US$)</t>
-  </si>
-  <si>
     <t>Female</t>
   </si>
   <si>
@@ -252,9 +247,6 @@
     <t>6_1</t>
   </si>
   <si>
-    <t>6_2</t>
-  </si>
-  <si>
     <t>7_1</t>
   </si>
   <si>
@@ -267,9 +259,6 @@
     <t>8_1</t>
   </si>
   <si>
-    <t>8_2</t>
-  </si>
-  <si>
     <t>Maternal Mortality</t>
   </si>
   <si>
@@ -319,12 +308,6 @@
   </si>
   <si>
     <t>%  of households with access</t>
-  </si>
-  <si>
-    <t>DOD, current US$</t>
-  </si>
-  <si>
-    <t>Use of IMF credit</t>
   </si>
   <si>
     <t>suffix</t>
@@ -627,7 +610,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="184">
+  <cellStyleXfs count="190">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -812,8 +795,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -829,7 +818,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -862,7 +850,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="184">
+  <cellStyles count="190">
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
@@ -953,6 +941,9 @@
     <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="181" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="183" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="185" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="187" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="189" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -1043,6 +1034,9 @@
     <cellStyle name="Hyperlink" xfId="178" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="180" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="182" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="184" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="186" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="188" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="23"/>
@@ -1375,645 +1369,600 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10:I10"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="42" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" style="14" bestFit="1" customWidth="1"/>
     <col min="7" max="10" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
+        <v>111</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="J3" s="15"/>
+        <v>59</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="J3" s="14"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="C4" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="G4" s="15" t="s">
+      <c r="B4" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
+      <c r="C4" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="J5" s="15"/>
+      <c r="B5" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="J5" s="14"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="B6" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="I6" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="J6" s="15"/>
+      <c r="C6" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B7" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="B7" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="I7" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="J7" s="15" t="s">
-        <v>130</v>
+      <c r="C7" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="C8" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="I8" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="J8" s="15"/>
+      <c r="B8" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="J8" s="14"/>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="C9" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="G9" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="I9" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="J9" s="15"/>
+      <c r="B9" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="J9" s="14"/>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>145</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="G10" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="H10" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
+        <v>140</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="C11" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="C11" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="E11" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="G11" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
+      <c r="G11" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="C12" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="F12" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="E12" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
+      <c r="G12" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>66</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="C13" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
+      <c r="D13" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>67</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="H14" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
+        <v>66</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>68</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="H15" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
+        <v>67</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>69</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="G16" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="H16" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="I16" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="J16" s="15"/>
+        <v>68</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="I16" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="J16" s="14"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>70</v>
-      </c>
-      <c r="B17" s="16"/>
-      <c r="D17" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
+        <v>69</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>71</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="F18" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="G18" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
+        <v>70</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>72</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="C19" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="D19" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="F19" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="G19" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="H19" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
+      <c r="C19" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>73</v>
-      </c>
-      <c r="B20" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="C20" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="G20" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
+      <c r="D20" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" t="s">
-        <v>74</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="F21" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="G21" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
+      <c r="B21" s="15"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" t="s">
-        <v>75</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="F22" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="G22" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
+      <c r="B22" s="15"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="B23" s="16"/>
+      <c r="B23" s="15"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="B24" s="16"/>
+      <c r="B24" s="15"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="B25" s="16"/>
+      <c r="B25" s="15"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="B26" s="16"/>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="B27" s="16"/>
-    </row>
-    <row r="28" spans="1:10">
-      <c r="B28" s="16"/>
+      <c r="B26" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2031,7 +1980,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2042,18 +1991,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>148</v>
+        <v>142</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B2">
         <v>17</v>
@@ -2064,7 +2013,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B3">
         <v>34</v>
@@ -2075,7 +2024,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B4">
         <v>29</v>
@@ -2086,7 +2035,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B5">
         <f>SUM(B2:B4)</f>
@@ -2113,7 +2062,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2130,7 +2079,7 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="20">
+      <c r="A2" s="19">
         <v>2002</v>
       </c>
       <c r="B2" s="5">
@@ -2138,7 +2087,7 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="20">
+      <c r="A3" s="19">
         <v>2003</v>
       </c>
       <c r="B3" s="5">
@@ -2146,7 +2095,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="20">
+      <c r="A4" s="19">
         <v>2004</v>
       </c>
       <c r="B4" s="5">
@@ -2154,7 +2103,7 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="20">
+      <c r="A5" s="19">
         <v>2005</v>
       </c>
       <c r="B5" s="5">
@@ -2162,7 +2111,7 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="20">
+      <c r="A6" s="19">
         <v>2006</v>
       </c>
       <c r="B6" s="5">
@@ -2170,7 +2119,7 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="20">
+      <c r="A7" s="19">
         <v>2007</v>
       </c>
       <c r="B7" s="5">
@@ -2178,7 +2127,7 @@
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="20">
+      <c r="A8" s="19">
         <v>2008</v>
       </c>
       <c r="B8" s="5">
@@ -2186,7 +2135,7 @@
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="20">
+      <c r="A9" s="19">
         <v>2009</v>
       </c>
       <c r="B9" s="5">
@@ -2194,7 +2143,7 @@
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="20">
+      <c r="A10" s="19">
         <v>2010</v>
       </c>
       <c r="B10" s="5">
@@ -2202,7 +2151,7 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="20">
+      <c r="A11" s="19">
         <v>2011</v>
       </c>
       <c r="B11" s="5">
@@ -2210,7 +2159,7 @@
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="20">
+      <c r="A12" s="19">
         <v>2012</v>
       </c>
       <c r="B12" s="5">
@@ -2250,7 +2199,7 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="20">
+      <c r="A2" s="19">
         <v>2002</v>
       </c>
       <c r="B2" s="5">
@@ -2258,7 +2207,7 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="20">
+      <c r="A3" s="19">
         <v>2003</v>
       </c>
       <c r="B3" s="5">
@@ -2266,7 +2215,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="20">
+      <c r="A4" s="19">
         <v>2004</v>
       </c>
       <c r="B4" s="6">
@@ -2275,7 +2224,7 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="20">
+      <c r="A5" s="19">
         <v>2005</v>
       </c>
       <c r="B5" s="5">
@@ -2283,7 +2232,7 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="20">
+      <c r="A6" s="19">
         <v>2006</v>
       </c>
       <c r="B6" s="5">
@@ -2291,7 +2240,7 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="20">
+      <c r="A7" s="19">
         <v>2007</v>
       </c>
       <c r="B7" s="5">
@@ -2299,7 +2248,7 @@
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="20">
+      <c r="A8" s="19">
         <v>2008</v>
       </c>
       <c r="B8" s="5">
@@ -2307,7 +2256,7 @@
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="20">
+      <c r="A9" s="19">
         <v>2009</v>
       </c>
       <c r="B9" s="6">
@@ -2316,7 +2265,7 @@
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="20">
+      <c r="A10" s="19">
         <v>2010</v>
       </c>
       <c r="B10" s="6">
@@ -2325,7 +2274,7 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="20">
+      <c r="A11" s="19">
         <v>2011</v>
       </c>
       <c r="B11" s="5">
@@ -2345,114 +2294,128 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="14">
+    <row r="1" spans="1:2" ht="30">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B2" s="5">
+        <v>29.909275198564355</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1">
+        <v>2001</v>
+      </c>
+      <c r="B3" s="5">
+        <v>12.633281115771387</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1">
+        <v>2002</v>
+      </c>
+      <c r="B4" s="5">
+        <v>19.779039868893221</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1">
         <v>2003</v>
       </c>
-      <c r="C1" s="14">
+      <c r="B5" s="5">
+        <v>21.92158336464988</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1">
+        <v>2004</v>
+      </c>
+      <c r="B6" s="5">
+        <v>9.6977533538063678</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1">
+        <v>2005</v>
+      </c>
+      <c r="B7" s="5">
+        <v>6.8832599118942728</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1">
+        <v>2006</v>
+      </c>
+      <c r="B8" s="5">
+        <v>7.0412617941135052</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1">
+        <v>2007</v>
+      </c>
+      <c r="B9" s="5">
+        <v>10.7696726019529</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1">
+        <v>2008</v>
+      </c>
+      <c r="B10" s="5">
+        <v>28.390943289090782</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1">
         <v>2009</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="19">
-        <v>90.8</v>
-      </c>
-      <c r="C2" s="19">
-        <v>88.8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="19">
-        <v>97</v>
-      </c>
-      <c r="C3" s="19">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="19">
-        <v>97.8</v>
-      </c>
-      <c r="C4" s="19">
-        <v>96.7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="19">
-        <v>96.2</v>
-      </c>
-      <c r="C5" s="19">
-        <v>97.399999999999991</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="19">
-        <v>97.6</v>
-      </c>
-      <c r="C6" s="19">
-        <v>97.8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="19">
-        <v>98.7</v>
-      </c>
-      <c r="C7" s="19">
-        <v>96.7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="19">
-        <v>96.2</v>
-      </c>
-      <c r="C8" s="19">
-        <v>95.199999999999989</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="19">
-        <v>97.2</v>
-      </c>
-      <c r="C9" s="19">
-        <v>94.899999999999991</v>
+      <c r="B11" s="5">
+        <v>43.293166895158379</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1">
+        <v>2010</v>
+      </c>
+      <c r="B12" s="5">
+        <v>7.2682341825053607</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1">
+        <v>2011</v>
+      </c>
+      <c r="B13" s="5">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="1">
+        <v>2012</v>
+      </c>
+      <c r="B14" s="5">
+        <v>16.2</v>
       </c>
     </row>
   </sheetData>
@@ -2468,128 +2431,114 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="30">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1">
-        <v>2000</v>
-      </c>
-      <c r="B2" s="5">
-        <v>29.909275198564355</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1">
-        <v>2001</v>
-      </c>
-      <c r="B3" s="5">
-        <v>12.633281115771387</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1">
-        <v>2002</v>
-      </c>
-      <c r="B4" s="5">
-        <v>19.779039868893221</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1">
+    <row r="1" spans="1:3">
+      <c r="A1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="13">
         <v>2003</v>
       </c>
-      <c r="B5" s="5">
-        <v>21.92158336464988</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="1">
-        <v>2004</v>
-      </c>
-      <c r="B6" s="5">
-        <v>9.6977533538063678</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1">
-        <v>2005</v>
-      </c>
-      <c r="B7" s="5">
-        <v>6.8832599118942728</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="1">
-        <v>2006</v>
-      </c>
-      <c r="B8" s="5">
-        <v>7.0412617941135052</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="1">
-        <v>2007</v>
-      </c>
-      <c r="B9" s="5">
-        <v>10.7696726019529</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="1">
-        <v>2008</v>
-      </c>
-      <c r="B10" s="5">
-        <v>28.390943289090782</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="1">
+      <c r="C1" s="13">
         <v>2009</v>
       </c>
-      <c r="B11" s="5">
-        <v>43.293166895158379</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="1">
-        <v>2010</v>
-      </c>
-      <c r="B12" s="5">
-        <v>7.2682341825053607</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="1">
-        <v>2011</v>
-      </c>
-      <c r="B13" s="5">
-        <v>7.2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="1">
-        <v>2012</v>
-      </c>
-      <c r="B14" s="5">
-        <v>16.2</v>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="18">
+        <v>90.8</v>
+      </c>
+      <c r="C2" s="18">
+        <v>88.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="18">
+        <v>97</v>
+      </c>
+      <c r="C3" s="18">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="18">
+        <v>97.8</v>
+      </c>
+      <c r="C4" s="18">
+        <v>96.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="18">
+        <v>96.2</v>
+      </c>
+      <c r="C5" s="18">
+        <v>97.399999999999991</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="18">
+        <v>97.6</v>
+      </c>
+      <c r="C6" s="18">
+        <v>97.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="18">
+        <v>98.7</v>
+      </c>
+      <c r="C7" s="18">
+        <v>96.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="18">
+        <v>96.2</v>
+      </c>
+      <c r="C8" s="18">
+        <v>95.199999999999989</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="18">
+        <v>97.2</v>
+      </c>
+      <c r="C9" s="18">
+        <v>94.899999999999991</v>
       </c>
     </row>
   </sheetData>
@@ -2617,101 +2566,101 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="14">
+      <c r="B1" s="13">
         <v>2003</v>
       </c>
-      <c r="C1" s="14">
+      <c r="C1" s="13">
         <v>2009</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="19">
+      <c r="B2" s="18">
         <v>1.7000000000000002</v>
       </c>
-      <c r="C2" s="19">
+      <c r="C2" s="18">
         <v>1.5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="18">
         <v>12.3</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="18">
         <v>14.2</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="18">
         <v>34.799999999999997</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="18">
         <v>34.9</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="18">
         <v>44.800000000000004</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="18">
         <v>50.2</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="18">
         <v>64.099999999999994</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="18">
         <v>57.9</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="18">
         <v>56.2</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="18">
         <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="18">
         <v>53.800000000000004</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="18">
         <v>52.7</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="18">
         <v>35</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="18">
         <v>35.199999999999996</v>
       </c>
     </row>
@@ -2731,7 +2680,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2819,14 +2768,79 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1">
+        <v>2004</v>
+      </c>
+      <c r="B2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1">
+        <v>2005</v>
+      </c>
+      <c r="B3">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1">
+        <v>2006</v>
+      </c>
+      <c r="B4">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1">
+        <v>2007</v>
+      </c>
+      <c r="B5">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1">
+        <v>2008</v>
+      </c>
+      <c r="B6">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1">
+        <v>2009</v>
+      </c>
+      <c r="B7">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1">
+        <v>2010</v>
+      </c>
+      <c r="B8">
+        <v>2253</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -2838,76 +2852,155 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>84</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="1">
+        <v>2001</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1.3903743315507999</v>
+      </c>
+      <c r="C2" s="5">
+        <v>23.9322062020224</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1">
+        <v>2002</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1.39973082099596</v>
+      </c>
+      <c r="C3" s="5">
+        <v>24.113449541037401</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
+        <v>2003</v>
+      </c>
+      <c r="B4" s="5">
+        <v>1.4325068870523401</v>
+      </c>
+      <c r="C4" s="5">
+        <v>23.821357364567199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
         <v>2004</v>
       </c>
-      <c r="B2">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1">
+      <c r="B5" s="5">
+        <v>2.7682508574228302</v>
+      </c>
+      <c r="C5" s="5">
+        <v>24.1340899309305</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
         <v>2005</v>
       </c>
-      <c r="B3">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1">
+      <c r="B6" s="5">
+        <v>2.5123373710183898</v>
+      </c>
+      <c r="C6" s="5">
+        <v>22.917450429550598</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1">
         <v>2006</v>
       </c>
-      <c r="B4">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1">
+      <c r="B7" s="5">
+        <v>2.27785295444294</v>
+      </c>
+      <c r="C7" s="5">
+        <v>22.149893990974402</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1">
         <v>2007</v>
       </c>
-      <c r="B5">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="1">
+      <c r="B8" s="5">
+        <v>1.9441571871768399</v>
+      </c>
+      <c r="C8" s="5">
+        <v>21.209074796302001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1">
         <v>2008</v>
       </c>
-      <c r="B6">
-        <v>1183</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1">
+      <c r="B9" s="5">
+        <v>1.47229755908563</v>
+      </c>
+      <c r="C9" s="5">
+        <v>20.584617744897201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1">
         <v>2009</v>
       </c>
-      <c r="B7">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="1">
+      <c r="B10" s="5">
+        <v>2.4115755627009601</v>
+      </c>
+      <c r="C10" s="5">
+        <v>20.944561864747001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1">
         <v>2010</v>
       </c>
-      <c r="B8">
-        <v>2253</v>
+      <c r="B11" s="5">
+        <v>3.0379256965944301</v>
+      </c>
+      <c r="C11" s="5">
+        <v>20.945424102329302</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1">
+        <v>2011</v>
+      </c>
+      <c r="B12" s="5">
+        <v>1.81003275297363</v>
+      </c>
+      <c r="C12" s="5">
+        <v>19.743536003779099</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1">
+        <v>2012</v>
+      </c>
+      <c r="B13" s="5">
+        <v>1.61534578495709</v>
+      </c>
+      <c r="C13" s="5">
+        <v>20.890055718429601</v>
       </c>
     </row>
   </sheetData>
@@ -2921,278 +3014,6 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1">
-        <v>2001</v>
-      </c>
-      <c r="B2" s="5">
-        <v>1.3903743315507999</v>
-      </c>
-      <c r="C2" s="5">
-        <v>23.9322062020224</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1">
-        <v>2002</v>
-      </c>
-      <c r="B3" s="5">
-        <v>1.39973082099596</v>
-      </c>
-      <c r="C3" s="5">
-        <v>24.113449541037401</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1">
-        <v>2003</v>
-      </c>
-      <c r="B4" s="5">
-        <v>1.4325068870523401</v>
-      </c>
-      <c r="C4" s="5">
-        <v>23.821357364567199</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1">
-        <v>2004</v>
-      </c>
-      <c r="B5" s="5">
-        <v>2.7682508574228302</v>
-      </c>
-      <c r="C5" s="5">
-        <v>24.1340899309305</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1">
-        <v>2005</v>
-      </c>
-      <c r="B6" s="5">
-        <v>2.5123373710183898</v>
-      </c>
-      <c r="C6" s="5">
-        <v>22.917450429550598</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1">
-        <v>2006</v>
-      </c>
-      <c r="B7" s="5">
-        <v>2.27785295444294</v>
-      </c>
-      <c r="C7" s="5">
-        <v>22.149893990974402</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1">
-        <v>2007</v>
-      </c>
-      <c r="B8" s="5">
-        <v>1.9441571871768399</v>
-      </c>
-      <c r="C8" s="5">
-        <v>21.209074796302001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="1">
-        <v>2008</v>
-      </c>
-      <c r="B9" s="5">
-        <v>1.47229755908563</v>
-      </c>
-      <c r="C9" s="5">
-        <v>20.584617744897201</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="1">
-        <v>2009</v>
-      </c>
-      <c r="B10" s="5">
-        <v>2.4115755627009601</v>
-      </c>
-      <c r="C10" s="5">
-        <v>20.944561864747001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="1">
-        <v>2010</v>
-      </c>
-      <c r="B11" s="5">
-        <v>3.0379256965944301</v>
-      </c>
-      <c r="C11" s="5">
-        <v>20.945424102329302</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="1">
-        <v>2011</v>
-      </c>
-      <c r="B12" s="5">
-        <v>1.81003275297363</v>
-      </c>
-      <c r="C12" s="5">
-        <v>19.743536003779099</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="1">
-        <v>2012</v>
-      </c>
-      <c r="B13" s="5">
-        <v>1.61534578495709</v>
-      </c>
-      <c r="C13" s="5">
-        <v>20.890055718429601</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="9.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1">
-        <v>2003</v>
-      </c>
-      <c r="B2" s="5">
-        <v>37.700000000000003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1">
-        <v>2004</v>
-      </c>
-      <c r="B3" s="5">
-        <v>43.7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1">
-        <v>2005</v>
-      </c>
-      <c r="B4" s="5">
-        <v>34.799999999999997</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1">
-        <v>2006</v>
-      </c>
-      <c r="B5" s="5">
-        <v>45.1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1">
-        <v>2007</v>
-      </c>
-      <c r="B6" s="6">
-        <f>B5*((B$8/B$5)^(1/3))</f>
-        <v>41.246844203018973</v>
-      </c>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1">
-        <v>2008</v>
-      </c>
-      <c r="B7" s="6">
-        <f>B6*((B$8/B$5)^(1/3))</f>
-        <v>37.722885958051435</v>
-      </c>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1">
-        <v>2009</v>
-      </c>
-      <c r="B8" s="5">
-        <v>34.5</v>
-      </c>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="1">
-        <v>2010</v>
-      </c>
-      <c r="B9" s="5">
-        <v>29.2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="1">
-        <v>2011</v>
-      </c>
-      <c r="B10" s="5">
-        <v>29.7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -3210,7 +3031,7 @@
         <v>27</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3264,114 +3085,102 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="9.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="B1" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="1">
+        <v>2003</v>
+      </c>
+      <c r="B2" s="5">
+        <v>37.700000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1">
         <v>2004</v>
       </c>
-      <c r="B2" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1">
+      <c r="B3" s="5">
+        <v>43.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
         <v>2005</v>
       </c>
-      <c r="B3" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1">
+      <c r="B4" s="5">
+        <v>34.799999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
         <v>2006</v>
       </c>
-      <c r="B4" s="6">
-        <f>B3*((B6/B3)^(1/3))</f>
-        <v>14.437863318006109</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1">
+      <c r="B5" s="5">
+        <v>45.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
         <v>2007</v>
       </c>
-      <c r="B5" s="6">
-        <f>B4*((B6/B3)^(1/3))</f>
-        <v>17.370991432452197</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="1">
+      <c r="B6" s="6">
+        <f>B5*((B$8/B$5)^(1/3))</f>
+        <v>41.246844203018973</v>
+      </c>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1">
         <v>2008</v>
       </c>
-      <c r="B6" s="5">
-        <v>20.9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1">
+      <c r="B7" s="6">
+        <f>B6*((B$8/B$5)^(1/3))</f>
+        <v>37.722885958051435</v>
+      </c>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1">
         <v>2009</v>
       </c>
-      <c r="B7" s="6">
-        <f>B6*((B9/B6)^(1/3))</f>
-        <v>29.200422993809891</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="1">
+      <c r="B8" s="5">
+        <v>34.5</v>
+      </c>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1">
         <v>2010</v>
       </c>
-      <c r="B8" s="6">
-        <f>B7*((B9/B6)^(1/3))</f>
-        <v>40.797354211359881</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="1">
+      <c r="B9" s="5">
+        <v>29.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1">
         <v>2011</v>
       </c>
-      <c r="B9" s="5">
-        <v>56.999999999999993</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="1">
-        <v>2012</v>
-      </c>
       <c r="B10" s="5">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="1">
-        <v>2013</v>
-      </c>
-      <c r="B11" s="5">
-        <v>76.599999999999994</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="1">
-        <v>2014</v>
-      </c>
-      <c r="B12" s="5">
-        <v>84</v>
+        <v>29.7</v>
       </c>
     </row>
   </sheetData>
@@ -3385,141 +3194,119 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>32</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1">
-        <v>2001</v>
-      </c>
-      <c r="B2" s="9">
-        <v>69583000</v>
+        <v>2004</v>
+      </c>
+      <c r="B2" s="5">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1">
-        <v>2002</v>
-      </c>
-      <c r="B3" s="9">
-        <v>75274000</v>
+        <v>2005</v>
+      </c>
+      <c r="B3" s="5">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1">
-        <v>2003</v>
-      </c>
-      <c r="B4" s="9">
-        <v>82276000</v>
+        <v>2006</v>
+      </c>
+      <c r="B4" s="6">
+        <f>B3*((B6/B3)^(1/3))</f>
+        <v>14.437863318006109</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1">
-        <v>2004</v>
-      </c>
-      <c r="B5" s="9">
-        <v>85988000</v>
+        <v>2007</v>
+      </c>
+      <c r="B5" s="6">
+        <f>B4*((B6/B3)^(1/3))</f>
+        <v>17.370991432452197</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1">
-        <v>2005</v>
-      </c>
-      <c r="B6" s="9">
-        <v>79136000</v>
+        <v>2008</v>
+      </c>
+      <c r="B6" s="5">
+        <v>20.9</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1">
-        <v>2006</v>
-      </c>
-      <c r="B7" s="9">
-        <v>83296000</v>
+        <v>2009</v>
+      </c>
+      <c r="B7" s="6">
+        <f>B6*((B9/B6)^(1/3))</f>
+        <v>29.200422993809891</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1">
-        <v>2007</v>
-      </c>
-      <c r="B8" s="9">
-        <v>87496000</v>
+        <v>2010</v>
+      </c>
+      <c r="B8" s="6">
+        <f>B7*((B9/B6)^(1/3))</f>
+        <v>40.797354211359881</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1">
-        <v>2008</v>
-      </c>
-      <c r="B9" s="9">
-        <v>85282000</v>
+        <v>2011</v>
+      </c>
+      <c r="B9" s="5">
+        <v>56.999999999999993</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1">
-        <v>2009</v>
-      </c>
-      <c r="B10" s="9">
-        <v>86801000</v>
+        <v>2012</v>
+      </c>
+      <c r="B10" s="5">
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1">
-        <v>2010</v>
-      </c>
-      <c r="B11" s="9">
-        <v>114160000</v>
+        <v>2013</v>
+      </c>
+      <c r="B11" s="5">
+        <v>76.599999999999994</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1">
-        <v>2011</v>
-      </c>
-      <c r="B12" s="9">
-        <v>113807000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="1">
-        <v>2012</v>
-      </c>
-      <c r="B13" s="9">
-        <v>234141000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="1">
-        <v>2013</v>
-      </c>
-      <c r="B14" s="9">
-        <v>230999000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="1">
         <v>2014</v>
       </c>
-      <c r="B15" s="9">
-        <v>203731000</v>
+      <c r="B12" s="5">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3533,7 +3320,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3546,13 +3333,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>34</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3745,7 +3532,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3755,7 +3542,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3889,7 +3676,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3899,13 +3686,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>37</v>
-      </c>
       <c r="D1" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -4004,10 +3791,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>36</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -4157,16 +3944,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -4372,7 +4159,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4385,13 +4172,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>34</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -4594,13 +4381,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:4">

</xml_diff>

<commit_message>
Added sorting of keys to allow starring for estimated years
</commit_message>
<xml_diff>
--- a/data/indicator_data.xlsx
+++ b/data/indicator_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="0" windowWidth="38400" windowHeight="19780" tabRatio="854" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14340" tabRatio="854" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="22" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="216">
   <si>
     <t>Year</t>
   </si>
@@ -658,6 +658,36 @@
   </si>
   <si>
     <t>#1BB0E8</t>
+  </si>
+  <si>
+    <t>2010*</t>
+  </si>
+  <si>
+    <t>2011*</t>
+  </si>
+  <si>
+    <t>2007*</t>
+  </si>
+  <si>
+    <t>2008*</t>
+  </si>
+  <si>
+    <t>2004*</t>
+  </si>
+  <si>
+    <t>2009*</t>
+  </si>
+  <si>
+    <t>2005*</t>
+  </si>
+  <si>
+    <t>2013*</t>
+  </si>
+  <si>
+    <t>2014*</t>
+  </si>
+  <si>
+    <t>2015*</t>
   </si>
 </sst>
 </file>
@@ -1606,7 +1636,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2474,7 +2504,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2507,8 +2537,8 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="19">
-        <v>2004</v>
+      <c r="A4" s="19" t="s">
+        <v>210</v>
       </c>
       <c r="B4" s="6">
         <f>B3*((B5/B3)^(1/2))</f>
@@ -2548,8 +2578,8 @@
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="19">
-        <v>2009</v>
+      <c r="A9" s="19" t="s">
+        <v>211</v>
       </c>
       <c r="B9" s="6">
         <f>B8*((B11/B8)^(1/3))</f>
@@ -2557,8 +2587,8 @@
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="19">
-        <v>2010</v>
+      <c r="A10" s="19" t="s">
+        <v>206</v>
       </c>
       <c r="B10" s="6">
         <f>B9*((B11/B8)^(1/3))</f>
@@ -2849,7 +2879,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C9"/>
+      <selection activeCell="N42" sqref="N42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3434,7 +3464,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3483,8 +3513,8 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="1">
-        <v>2007</v>
+      <c r="A6" s="1" t="s">
+        <v>208</v>
       </c>
       <c r="B6" s="6">
         <f>B5*((B$8/B$5)^(1/3))</f>
@@ -3493,8 +3523,8 @@
       <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="1">
-        <v>2008</v>
+      <c r="A7" s="1" t="s">
+        <v>209</v>
       </c>
       <c r="B7" s="6">
         <f>B6*((B$8/B$5)^(1/3))</f>
@@ -4161,8 +4191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4184,8 +4214,8 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="1">
-        <v>2004</v>
+      <c r="A3" s="1" t="s">
+        <v>210</v>
       </c>
       <c r="B3" s="27">
         <f>B2*((B5/B2)^(1/3))</f>
@@ -4193,8 +4223,8 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="1">
-        <v>2005</v>
+      <c r="A4" s="1" t="s">
+        <v>212</v>
       </c>
       <c r="B4" s="27">
         <f>B3*((B5/B2)^(1/3))</f>
@@ -4210,8 +4240,8 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="1">
-        <v>2007</v>
+      <c r="A6" s="1" t="s">
+        <v>208</v>
       </c>
       <c r="B6" s="27">
         <f>B5*((B8/B5)^(1/3))</f>
@@ -4219,8 +4249,8 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="1">
-        <v>2008</v>
+      <c r="A7" s="1" t="s">
+        <v>209</v>
       </c>
       <c r="B7" s="27">
         <f>B6*((B8/B5)^(1/3))</f>
@@ -4236,8 +4266,8 @@
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="1">
-        <v>2010</v>
+      <c r="A9" s="1" t="s">
+        <v>206</v>
       </c>
       <c r="B9" s="27">
         <f>B8*((B11/B8)^(1/3))</f>
@@ -4245,8 +4275,8 @@
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="1">
-        <v>2011</v>
+      <c r="A10" s="1" t="s">
+        <v>207</v>
       </c>
       <c r="B10" s="27">
         <f>B9*((B11/B8)^(1/3))</f>
@@ -4262,8 +4292,8 @@
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="1">
-        <v>2013</v>
+      <c r="A12" s="1" t="s">
+        <v>213</v>
       </c>
       <c r="B12" s="27">
         <f>B11*(1+0.11)</f>
@@ -4271,8 +4301,8 @@
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="1">
-        <v>2014</v>
+      <c r="A13" s="1" t="s">
+        <v>214</v>
       </c>
       <c r="B13" s="27">
         <f t="shared" ref="B13:B14" si="0">B12*(1+0.11)</f>
@@ -4280,8 +4310,8 @@
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="1">
-        <v>2015</v>
+      <c r="A14" s="1" t="s">
+        <v>215</v>
       </c>
       <c r="B14" s="27">
         <f t="shared" si="0"/>
@@ -4303,8 +4333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4439,8 +4469,8 @@
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="1">
-        <v>2010</v>
+      <c r="A10" s="1" t="s">
+        <v>206</v>
       </c>
       <c r="B10" s="6">
         <f>B9*((B$12/B$9)^(1/3))</f>
@@ -4456,8 +4486,8 @@
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="1">
-        <v>2011</v>
+      <c r="A11" s="1" t="s">
+        <v>207</v>
       </c>
       <c r="B11" s="6">
         <f>B10*((B$12/B$9)^(1/3))</f>
@@ -5143,7 +5173,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5278,8 +5308,8 @@
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="1">
-        <v>2010</v>
+      <c r="A10" s="1" t="s">
+        <v>206</v>
       </c>
       <c r="B10" s="6">
         <f>B9*((B$12/B$9)^(1/3))</f>
@@ -5295,8 +5325,8 @@
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="1">
-        <v>2011</v>
+      <c r="A11" s="1" t="s">
+        <v>207</v>
       </c>
       <c r="B11" s="6">
         <f>B10*((B$12/B$9)^(1/3))</f>

</xml_diff>

<commit_message>
Changed unit for gender enrolment ratios and fixed issue with rounding
</commit_message>
<xml_diff>
--- a/data/indicator_data.xlsx
+++ b/data/indicator_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14340" tabRatio="854" activeTab="21"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14340" tabRatio="854"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="22" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="217">
   <si>
     <t>Year</t>
   </si>
@@ -189,9 +189,6 @@
     <t>3_2</t>
   </si>
   <si>
-    <t xml:space="preserve"># of females as % of the # of males </t>
-  </si>
-  <si>
     <t>Gender Enrolment Ratios</t>
   </si>
   <si>
@@ -688,6 +685,12 @@
   </si>
   <si>
     <t>2015*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">females as % of the class </t>
+  </si>
+  <si>
+    <t>rounding</t>
   </si>
 </sst>
 </file>
@@ -818,7 +821,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="210">
+  <cellStyleXfs count="212">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -843,6 +846,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="166" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1094,7 +1099,7 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="210">
+  <cellStyles count="212">
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
@@ -1198,6 +1203,7 @@
     <cellStyle name="Followed Hyperlink" xfId="205" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="207" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="209" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="211" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -1301,6 +1307,7 @@
     <cellStyle name="Hyperlink" xfId="204" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="206" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="208" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="210" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="23"/>
@@ -1633,657 +1640,723 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="42" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.6640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="13.1640625" customWidth="1"/>
+    <col min="8" max="11" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E1" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="I1" s="8" t="s">
+      <c r="F2" s="14">
+        <v>1</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="H2" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="J1" s="8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>198</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="H2" s="14"/>
       <c r="I2" s="14"/>
       <c r="J2" s="14"/>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2" s="14"/>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>47</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>198</v>
+        <v>90</v>
+      </c>
+      <c r="F3" s="14">
+        <v>1</v>
       </c>
       <c r="G3" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="I3" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="H3" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="J3" s="14"/>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="J3" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="K3" s="14"/>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>198</v>
+        <v>94</v>
+      </c>
+      <c r="F4" s="14">
+        <v>1</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="H4" s="14"/>
+        <v>197</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>99</v>
+      </c>
       <c r="I4" s="14"/>
       <c r="J4" s="14"/>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="K4" s="14"/>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="F5" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" s="14">
+        <v>1</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="K5" s="14"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F6" s="14">
+        <v>0</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="K6" s="14"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7" s="14">
+        <v>1</v>
+      </c>
+      <c r="G7" s="14" t="s">
         <v>199</v>
       </c>
-      <c r="G5" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="I5" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="J5" s="14"/>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>199</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="J6" s="14"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>200</v>
-      </c>
-      <c r="G7" s="14" t="s">
+      <c r="H7" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="I7" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="J7" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="K7" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="J7" s="14" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>48</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>47</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>200</v>
+        <v>90</v>
+      </c>
+      <c r="F8" s="14">
+        <v>1</v>
       </c>
       <c r="G8" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="I8" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="J8" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="I8" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="J8" s="14"/>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="K8" s="14"/>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>46</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>45</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>200</v>
+        <v>94</v>
+      </c>
+      <c r="F9" s="14">
+        <v>1</v>
       </c>
       <c r="G9" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="I9" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="J9" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="I9" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="J9" s="14"/>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="K9" s="14"/>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B10" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="B10" s="15" t="s">
-        <v>133</v>
-      </c>
       <c r="C10" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>200</v>
+        <v>94</v>
+      </c>
+      <c r="F10" s="14">
+        <v>0</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>119</v>
+        <v>199</v>
       </c>
       <c r="H10" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="I10" s="14"/>
+      <c r="I10" s="14" t="s">
+        <v>117</v>
+      </c>
       <c r="J10" s="14"/>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="K10" s="14"/>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>44</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>201</v>
+        <v>94</v>
+      </c>
+      <c r="F11" s="14">
+        <v>1</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="H11" s="14"/>
+        <v>200</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>120</v>
+      </c>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="K11" s="14"/>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>43</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>201</v>
+        <v>94</v>
+      </c>
+      <c r="F12" s="14">
+        <v>1</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="H12" s="14"/>
+        <v>200</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>120</v>
+      </c>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="K12" s="14"/>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>202</v>
+        <v>94</v>
+      </c>
+      <c r="F13" s="14">
+        <v>1</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="H13" s="14"/>
+        <v>201</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>121</v>
+      </c>
       <c r="I13" s="14"/>
       <c r="J13" s="14"/>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="K13" s="14"/>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="F14" s="14">
+        <v>1</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="I14" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" t="s">
         <v>66</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B15" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="F14" s="14" t="s">
+      <c r="D15" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="F15" s="14">
+        <v>1</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="I15" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F16" s="14">
+        <v>0</v>
+      </c>
+      <c r="G16" s="14" t="s">
         <v>202</v>
       </c>
-      <c r="G14" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="F15" s="14" t="s">
+      <c r="H16" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="I16" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="K16" s="14"/>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" t="s">
+        <v>194</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F17" s="14">
+        <v>0</v>
+      </c>
+      <c r="G17" s="14" t="s">
         <v>202</v>
       </c>
-      <c r="G15" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="H15" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" t="s">
-        <v>68</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>203</v>
-      </c>
-      <c r="G16" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="H16" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="I16" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="J16" s="14"/>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" t="s">
-        <v>195</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>196</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>197</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>203</v>
-      </c>
-      <c r="G17" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="H17" s="14"/>
+      <c r="H17" s="14" t="s">
+        <v>123</v>
+      </c>
       <c r="I17" s="14"/>
       <c r="J17" s="14"/>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="K17" s="14"/>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>204</v>
+        <v>93</v>
+      </c>
+      <c r="F18" s="14">
+        <v>0</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="H18" s="14"/>
+        <v>203</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>129</v>
+      </c>
       <c r="I18" s="14"/>
       <c r="J18" s="14"/>
-    </row>
-    <row r="19" spans="1:10">
+      <c r="K18" s="14"/>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="F19" s="14">
+        <v>1</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="I19" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" t="s">
         <v>70</v>
       </c>
-      <c r="B19" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>204</v>
-      </c>
-      <c r="G19" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="H19" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" t="s">
-        <v>71</v>
-      </c>
       <c r="B20" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>204</v>
+        <v>94</v>
+      </c>
+      <c r="F20" s="14">
+        <v>0</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="H20" s="14"/>
+        <v>203</v>
+      </c>
+      <c r="H20" s="14" t="s">
+        <v>128</v>
+      </c>
       <c r="I20" s="14"/>
       <c r="J20" s="14"/>
-    </row>
-    <row r="21" spans="1:10">
+      <c r="K20" s="14"/>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" t="s">
+        <v>176</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="C21" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="B21" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="C21" s="14" t="s">
+      <c r="D21" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="F21" s="14">
+        <v>0</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="H21" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="D21" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="E21" s="14" t="s">
+      <c r="I21" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="J21" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="K21" s="14" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="E22" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="F22" s="14">
+        <v>1</v>
+      </c>
+      <c r="G22" s="14" t="s">
         <v>204</v>
       </c>
-      <c r="G21" s="14" t="s">
-        <v>179</v>
-      </c>
-      <c r="H21" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="I21" s="14" t="s">
-        <v>181</v>
-      </c>
-      <c r="J21" s="14" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" t="s">
-        <v>72</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>205</v>
-      </c>
-      <c r="G22" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="H22" s="14"/>
+      <c r="H22" s="14" t="s">
+        <v>122</v>
+      </c>
       <c r="I22" s="14"/>
       <c r="J22" s="14"/>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="K22" s="14"/>
+    </row>
+    <row r="23" spans="1:11">
       <c r="B23" s="15"/>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:11">
       <c r="B24" s="15"/>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:11">
       <c r="B25" s="15"/>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:11">
       <c r="B26" s="15"/>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:11">
       <c r="B27" s="15"/>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:11">
       <c r="B28" s="15"/>
     </row>
   </sheetData>
@@ -2313,18 +2386,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>134</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B2">
         <v>17</v>
@@ -2335,7 +2408,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B3">
         <v>34</v>
@@ -2346,7 +2419,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B4">
         <v>29</v>
@@ -2357,7 +2430,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B5">
         <f>SUM(B2:B4)</f>
@@ -2504,7 +2577,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2538,7 +2611,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B4" s="6">
         <f>B3*((B5/B3)^(1/2))</f>
@@ -2579,7 +2652,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="19" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B9" s="6">
         <f>B8*((B11/B8)^(1/3))</f>
@@ -2588,7 +2661,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B10" s="6">
         <f>B9*((B11/B8)^(1/3))</f>
@@ -3100,15 +3173,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="26" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B2">
         <v>51</v>
@@ -3116,7 +3189,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B3">
         <v>47</v>
@@ -3124,7 +3197,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B4">
         <v>27</v>
@@ -3132,7 +3205,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B5">
         <v>22</v>
@@ -3140,7 +3213,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B6">
         <v>18</v>
@@ -3148,7 +3221,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B7">
         <v>17</v>
@@ -3156,7 +3229,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B8">
         <v>14</v>
@@ -3164,7 +3237,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -3172,7 +3245,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B10">
         <v>5</v>
@@ -3203,7 +3276,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3311,10 +3384,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -3514,7 +3587,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B6" s="6">
         <f>B5*((B$8/B$5)^(1/3))</f>
@@ -3524,7 +3597,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B7" s="6">
         <f>B6*((B$8/B$5)^(1/3))</f>
@@ -3586,7 +3659,7 @@
         <v>27</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3652,24 +3725,24 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="C1" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="D1" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="C1" s="21" t="s">
-        <v>176</v>
-      </c>
-      <c r="D1" s="21" t="s">
+      <c r="E1" s="21" t="s">
         <v>144</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B2" s="23">
         <v>34574</v>
@@ -3686,7 +3759,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="22" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B3" s="24">
         <v>34193</v>
@@ -3703,7 +3776,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B4" s="23">
         <v>31274</v>
@@ -3720,7 +3793,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B5" s="23">
         <v>23296</v>
@@ -3737,7 +3810,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B6" s="23">
         <v>25259</v>
@@ -3754,7 +3827,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B7" s="23">
         <v>23273</v>
@@ -3771,7 +3844,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B8" s="23">
         <v>29006</v>
@@ -3788,7 +3861,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B9" s="23">
         <v>24843</v>
@@ -3805,7 +3878,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B10" s="23">
         <v>23233</v>
@@ -3822,7 +3895,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B11" s="23">
         <v>34430</v>
@@ -3839,7 +3912,7 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B12" s="23">
         <v>24686</v>
@@ -3856,7 +3929,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B13" s="23">
         <v>20553</v>
@@ -3873,7 +3946,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B14" s="23">
         <v>15860</v>
@@ -3890,7 +3963,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B15" s="23">
         <v>19373</v>
@@ -3907,7 +3980,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B16" s="23">
         <v>21756</v>
@@ -3924,7 +3997,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B17" s="23">
         <v>19769</v>
@@ -3941,7 +4014,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B18" s="23">
         <v>16894</v>
@@ -3958,7 +4031,7 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B19" s="23">
         <v>10133</v>
@@ -3975,7 +4048,7 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B20" s="23">
         <v>17767</v>
@@ -3992,7 +4065,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B21" s="23">
         <v>15672</v>
@@ -4009,7 +4082,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B22" s="23">
         <v>10497</v>
@@ -4026,7 +4099,7 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B23" s="23">
         <v>17854</v>
@@ -4043,7 +4116,7 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B24" s="23">
         <v>18344</v>
@@ -4060,7 +4133,7 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B25" s="23">
         <v>15512</v>
@@ -4077,7 +4150,7 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B26" s="23">
         <v>13651</v>
@@ -4094,7 +4167,7 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B27" s="23">
         <v>6449</v>
@@ -4111,7 +4184,7 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B28" s="23">
         <v>5379</v>
@@ -4128,7 +4201,7 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B29" s="23">
         <v>8575</v>
@@ -4145,7 +4218,7 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B30" s="23">
         <v>7128</v>
@@ -4162,7 +4235,7 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B31" s="23">
         <v>4998</v>
@@ -4191,7 +4264,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -4202,7 +4275,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -4215,7 +4288,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B3" s="27">
         <f>B2*((B5/B2)^(1/3))</f>
@@ -4224,7 +4297,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B4" s="27">
         <f>B3*((B5/B2)^(1/3))</f>
@@ -4241,7 +4314,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B6" s="27">
         <f>B5*((B8/B5)^(1/3))</f>
@@ -4250,7 +4323,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B7" s="27">
         <f>B6*((B8/B5)^(1/3))</f>
@@ -4267,7 +4340,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B9" s="27">
         <f>B8*((B11/B8)^(1/3))</f>
@@ -4276,7 +4349,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B10" s="27">
         <f>B9*((B11/B8)^(1/3))</f>
@@ -4293,7 +4366,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B12" s="27">
         <f>B11*(1+0.11)</f>
@@ -4302,7 +4375,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B13" s="27">
         <f t="shared" ref="B13:B14" si="0">B12*(1+0.11)</f>
@@ -4311,7 +4384,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B14" s="27">
         <f t="shared" si="0"/>
@@ -4470,7 +4543,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B10" s="6">
         <f>B9*((B$12/B$9)^(1/3))</f>
@@ -4487,7 +4560,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B11" s="6">
         <f>B10*((B$12/B$9)^(1/3))</f>
@@ -4948,7 +5021,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4975,16 +5048,16 @@
         <v>6</v>
       </c>
       <c r="B2" s="5">
-        <v>94.182217343578486</v>
+        <v>48.501978518937257</v>
       </c>
       <c r="C2" s="5">
-        <v>90.928819444444443</v>
+        <v>47.624460104569224</v>
       </c>
       <c r="D2" s="5">
-        <v>91.75168921888644</v>
+        <v>47.849220829627725</v>
       </c>
       <c r="E2" s="5">
-        <v>79.147406266050339</v>
+        <v>44.180045871559628</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -4992,16 +5065,16 @@
         <v>7</v>
       </c>
       <c r="B3" s="5">
-        <v>101.97706603400553</v>
+        <v>50.489428347689902</v>
       </c>
       <c r="C3" s="5">
-        <v>92.325516730002775</v>
+        <v>48.004819277108432</v>
       </c>
       <c r="D3" s="5">
-        <v>92.401404581611445</v>
+        <v>48.02532745670122</v>
       </c>
       <c r="E3" s="5">
-        <v>75.628831113929408</v>
+        <v>43.061740281622335</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -5009,16 +5082,16 @@
         <v>8</v>
       </c>
       <c r="B4" s="5">
-        <v>87.90922619047619</v>
+        <v>46.782815284102156</v>
       </c>
       <c r="C4" s="5">
-        <v>93.725886459672964</v>
+        <v>48.38067238844895</v>
       </c>
       <c r="D4" s="5">
-        <v>92.759079356784881</v>
+        <v>48.121769239774011</v>
       </c>
       <c r="E4" s="5">
-        <v>76.992616244262621</v>
+        <v>43.500467916699556</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -5026,16 +5099,16 @@
         <v>9</v>
       </c>
       <c r="B5" s="5">
-        <v>81.374389785955685</v>
+        <v>44.865424430641824</v>
       </c>
       <c r="C5" s="5">
-        <v>104.6077210460772</v>
+        <v>51.125989044430916</v>
       </c>
       <c r="D5" s="5">
-        <v>93.127628904957703</v>
+        <v>48.220769567252248</v>
       </c>
       <c r="E5" s="5">
-        <v>79.516417910447757</v>
+        <v>44.294788652765305</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -5043,16 +5116,16 @@
         <v>10</v>
       </c>
       <c r="B6" s="5">
-        <v>84.925535779150024</v>
+        <v>45.92417992535848</v>
       </c>
       <c r="C6" s="5">
-        <v>89.336926186122611</v>
+        <v>47.184100843753178</v>
       </c>
       <c r="D6" s="5">
-        <v>90.764060340448665</v>
+        <v>47.579224398173231</v>
       </c>
       <c r="E6" s="5">
-        <v>81.878699623654896</v>
+        <v>45.018300544857134</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -5060,16 +5133,16 @@
         <v>1</v>
       </c>
       <c r="B7" s="5">
-        <v>83.086375135525842</v>
+        <v>45.380971180418477</v>
       </c>
       <c r="C7" s="5">
-        <v>96.440032089851584</v>
+        <v>49.093879217928425</v>
       </c>
       <c r="D7" s="5">
-        <v>91.8105914709556</v>
+        <v>47.865235577910084</v>
       </c>
       <c r="E7" s="5">
-        <v>80.234531975334306</v>
+        <v>44.516736663046721</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -5077,16 +5150,16 @@
         <v>2</v>
       </c>
       <c r="B8" s="5">
-        <v>92.098397316436817</v>
+        <v>47.943344974776878</v>
       </c>
       <c r="C8" s="5">
-        <v>94.161419576416719</v>
+        <v>48.496462264150942</v>
       </c>
       <c r="D8" s="5">
-        <v>93.297428992755016</v>
+        <v>48.266254486112125</v>
       </c>
       <c r="E8" s="5">
-        <v>83.264774441245024</v>
+        <v>45.43414013691968</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -5094,16 +5167,16 @@
         <v>3</v>
       </c>
       <c r="B9" s="5">
-        <v>90.313075506445671</v>
+        <v>47.455002903038512</v>
       </c>
       <c r="C9" s="5">
-        <v>96.798292422625394</v>
+        <v>49.186550976138825</v>
       </c>
       <c r="D9" s="5">
-        <v>93.697346665616877</v>
+        <v>48.373066682925838</v>
       </c>
       <c r="E9" s="5">
-        <v>85.010910602334519</v>
+        <v>45.949133662207828</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -5111,16 +5184,16 @@
         <v>4</v>
       </c>
       <c r="B10" s="5">
-        <v>87.835482746601599</v>
+        <v>46.761922434588975</v>
       </c>
       <c r="C10" s="5">
-        <v>95.506158583525789</v>
+        <v>48.850716149037751</v>
       </c>
       <c r="D10" s="5">
-        <v>93.697346665616877</v>
+        <v>48.373066682925838</v>
       </c>
       <c r="E10" s="5">
-        <v>85.292863235712261</v>
+        <v>46.031380672881426</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -5128,16 +5201,16 @@
         <v>5</v>
       </c>
       <c r="B11" s="5">
-        <v>95.289855072463766</v>
+        <v>48.794063079777366</v>
       </c>
       <c r="C11" s="5">
-        <v>92.310459573702673</v>
+        <v>48.000748257961931</v>
       </c>
       <c r="D11" s="5">
-        <v>93.028717913188075</v>
+        <v>48.194237064262339</v>
       </c>
       <c r="E11" s="5">
-        <v>87.106350995866208</v>
+        <v>46.554459820442268</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -5145,16 +5218,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="5">
-        <v>92.551020408163268</v>
+        <v>48.065712771595123</v>
       </c>
       <c r="C12" s="5">
-        <v>94.23110643520954</v>
+        <v>48.514940868466191</v>
       </c>
       <c r="D12" s="5">
-        <v>93.846339113680159</v>
+        <v>48.412747716965896</v>
       </c>
       <c r="E12" s="5">
-        <v>88.674101610904586</v>
+        <v>46.998555103113091</v>
       </c>
     </row>
   </sheetData>
@@ -5309,7 +5382,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B10" s="6">
         <f>B9*((B$12/B$9)^(1/3))</f>
@@ -5326,7 +5399,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B11" s="6">
         <f>B10*((B$12/B$9)^(1/3))</f>

</xml_diff>

<commit_message>
Update to numerical values
</commit_message>
<xml_diff>
--- a/data/indicator_data.xlsx
+++ b/data/indicator_data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26812"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27106"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" tabRatio="854"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" tabRatio="854" firstSheet="9" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="22" r:id="rId1"/>
@@ -39,6 +39,9 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -771,7 +774,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="#.00;\-#.00;0.00;@"/>
-    <numFmt numFmtId="168" formatCode="#,##0.0"/>
+    <numFmt numFmtId="167" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -1169,11 +1172,11 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1738,7 +1741,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
@@ -3908,7 +3911,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4777,8 +4780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4882,8 +4885,8 @@
         <v>191</v>
       </c>
       <c r="B12" s="26">
-        <f>B11*(1+0.11)</f>
-        <v>68.820000000000007</v>
+        <f>B11*(B11/B10)</f>
+        <v>68.989778099448955</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -4891,8 +4894,8 @@
         <v>192</v>
       </c>
       <c r="B13" s="26">
-        <f t="shared" ref="B13:B14" si="0">B12*(1+0.11)</f>
-        <v>76.390200000000021</v>
+        <f t="shared" ref="B13:B14" si="0">B12*(B12/B11)</f>
+        <v>76.767572293729145</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -4901,7 +4904,7 @@
       </c>
       <c r="B14" s="26">
         <f t="shared" si="0"/>
-        <v>84.793122000000025</v>
+        <v>85.422222222222246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>